<commit_message>
added env and files
</commit_message>
<xml_diff>
--- a/Warehouse.xlsx
+++ b/Warehouse.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erikwahlstrom/Performance_Engineering/assignment4-construction-project/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBFB3B91-17D1-C34D-88F3-5C250B31D857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -28,143 +34,143 @@
     <t>Duration</t>
   </si>
   <si>
+    <t>Early Start Date</t>
+  </si>
+  <si>
+    <t>Early Completion Date</t>
+  </si>
+  <si>
+    <t>Late Start Date</t>
+  </si>
+  <si>
+    <t>Late Completion Date</t>
+  </si>
+  <si>
+    <t>Critcal Task?</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>End</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>['Start']</t>
+  </si>
+  <si>
+    <t>['A']</t>
+  </si>
+  <si>
+    <t>['A', 'B']</t>
+  </si>
+  <si>
+    <t>['C']</t>
+  </si>
+  <si>
+    <t>['D', 'F']</t>
+  </si>
+  <si>
+    <t>['E']</t>
+  </si>
+  <si>
+    <t>['G']</t>
+  </si>
+  <si>
+    <t>['H', 'J']</t>
+  </si>
+  <si>
+    <t>['K']</t>
+  </si>
+  <si>
+    <t>['C', 'D', 'E']</t>
+  </si>
+  <si>
+    <t>['D']</t>
+  </si>
+  <si>
+    <t>['F']</t>
+  </si>
+  <si>
+    <t>['H']</t>
+  </si>
+  <si>
+    <t>['J']</t>
+  </si>
+  <si>
+    <t>['End']</t>
+  </si>
+  <si>
+    <t>Agreement of the owner</t>
+  </si>
+  <si>
+    <t>Preparation of the ground</t>
+  </si>
+  <si>
+    <t>Order of materials</t>
+  </si>
+  <si>
+    <t>Excavation</t>
+  </si>
+  <si>
+    <t>Order of doors and windows</t>
+  </si>
+  <si>
+    <t>Delivery of materials</t>
+  </si>
+  <si>
+    <t>Concrete foundations</t>
+  </si>
+  <si>
+    <t>Delivery of doors and windows</t>
+  </si>
+  <si>
+    <t>Frame, roofs, walls</t>
+  </si>
+  <si>
+    <t>Installation of doors and windows</t>
+  </si>
+  <si>
     <t>Description</t>
-  </si>
-  <si>
-    <t>Early Start Date</t>
-  </si>
-  <si>
-    <t>Early Completion Date</t>
-  </si>
-  <si>
-    <t>Late Start Date</t>
-  </si>
-  <si>
-    <t>Late Completion Date</t>
-  </si>
-  <si>
-    <t>Critcal Task?</t>
-  </si>
-  <si>
-    <t>Start</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>J</t>
-  </si>
-  <si>
-    <t>K</t>
-  </si>
-  <si>
-    <t>End</t>
-  </si>
-  <si>
-    <t>[]</t>
-  </si>
-  <si>
-    <t>['Start']</t>
-  </si>
-  <si>
-    <t>['A']</t>
-  </si>
-  <si>
-    <t>['A', 'B']</t>
-  </si>
-  <si>
-    <t>['C']</t>
-  </si>
-  <si>
-    <t>['D', 'F']</t>
-  </si>
-  <si>
-    <t>['E']</t>
-  </si>
-  <si>
-    <t>['G']</t>
-  </si>
-  <si>
-    <t>['H', 'J']</t>
-  </si>
-  <si>
-    <t>['K']</t>
-  </si>
-  <si>
-    <t>['C', 'D', 'E']</t>
-  </si>
-  <si>
-    <t>['D']</t>
-  </si>
-  <si>
-    <t>['F']</t>
-  </si>
-  <si>
-    <t>['H']</t>
-  </si>
-  <si>
-    <t>['J']</t>
-  </si>
-  <si>
-    <t>['End']</t>
-  </si>
-  <si>
-    <t>Agreement of the owner</t>
-  </si>
-  <si>
-    <t>Preparation of the ground</t>
-  </si>
-  <si>
-    <t>Order of materials</t>
-  </si>
-  <si>
-    <t>Excavation</t>
-  </si>
-  <si>
-    <t>Order of doors and windows</t>
-  </si>
-  <si>
-    <t>Delivery of materials</t>
-  </si>
-  <si>
-    <t>Concrete foundations</t>
-  </si>
-  <si>
-    <t>Delivery of doors and windows</t>
-  </si>
-  <si>
-    <t>Frame, roofs, walls</t>
-  </si>
-  <si>
-    <t>Installation of doors and windows</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -227,6 +233,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -273,7 +287,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -305,9 +319,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -339,6 +371,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -514,14 +564,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -535,33 +587,33 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -582,21 +634,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D3">
         <v>4</v>
       </c>
       <c r="E3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -614,21 +666,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D4">
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -646,21 +698,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F5">
         <v>4</v>
@@ -678,21 +730,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F6">
         <v>4</v>
@@ -710,21 +762,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D7">
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F7">
         <v>4</v>
@@ -742,21 +794,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D8">
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F8">
         <v>5</v>
@@ -774,21 +826,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D9">
         <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F9">
         <v>7</v>
@@ -806,21 +858,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D10">
         <v>10</v>
       </c>
       <c r="E10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F10">
         <v>6</v>
@@ -838,21 +890,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D11">
         <v>4</v>
       </c>
       <c r="E11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F11">
         <v>9</v>
@@ -870,21 +922,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F12">
         <v>16</v>
@@ -902,15 +954,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" t="s">
         <v>21</v>
-      </c>
-      <c r="B13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" t="s">
-        <v>22</v>
       </c>
       <c r="D13">
         <v>0</v>

</xml_diff>